<commit_message>
Updated with new metadata
</commit_message>
<xml_diff>
--- a/Data/Myctophid_Catalog.xlsx
+++ b/Data/Myctophid_Catalog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1176,7 +1176,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1184,6 +1184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1466,28 +1467,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1571,13 +1572,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>80</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1647,25 +1648,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>339</v>
       </c>
       <c r="C14" s="1">
         <f>SUM(C4:C13)</f>
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D14" s="1">
         <f>SUM(D4:D13)</f>
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>348</v>
       </c>
@@ -1674,9 +1675,19 @@
         <v>380.6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>349</v>
+      </c>
+      <c r="B19" s="6">
+        <f>D14*8</f>
+        <v>880</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <f>SUM(B18:B19)</f>
+        <v>1260.5999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1692,17 +1703,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A180" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1737,7 +1748,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1772,7 +1783,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -1807,7 +1818,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -1842,7 +1853,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1877,7 +1888,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -1912,7 +1923,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1947,7 +1958,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -1982,7 +1993,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -2017,7 +2028,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -2052,7 +2063,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -2087,7 +2098,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -2122,7 +2133,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
@@ -2157,7 +2168,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>132</v>
       </c>
@@ -2192,7 +2203,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -2227,7 +2238,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -2262,7 +2273,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -2297,7 +2308,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>136</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -2402,7 +2413,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>139</v>
       </c>
@@ -2437,7 +2448,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -2472,7 +2483,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>141</v>
       </c>
@@ -2507,7 +2518,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>142</v>
       </c>
@@ -2542,7 +2553,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>143</v>
       </c>
@@ -2577,7 +2588,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -2612,7 +2623,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -2647,7 +2658,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -2682,7 +2693,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -2717,7 +2728,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -2752,7 +2763,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -2787,7 +2798,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>150</v>
       </c>
@@ -2822,7 +2833,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -2857,7 +2868,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -2892,7 +2903,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>153</v>
       </c>
@@ -2927,7 +2938,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>154</v>
       </c>
@@ -2962,7 +2973,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>155</v>
       </c>
@@ -2988,7 +2999,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>156</v>
       </c>
@@ -3023,7 +3034,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>157</v>
       </c>
@@ -3058,7 +3069,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>158</v>
       </c>
@@ -3093,7 +3104,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>159</v>
       </c>
@@ -3128,7 +3139,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>160</v>
       </c>
@@ -3163,7 +3174,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -3198,7 +3209,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>162</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>163</v>
       </c>
@@ -3268,7 +3279,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>164</v>
       </c>
@@ -3303,7 +3314,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>165</v>
       </c>
@@ -3338,7 +3349,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>166</v>
       </c>
@@ -3373,7 +3384,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>167</v>
       </c>
@@ -3408,7 +3419,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>168</v>
       </c>
@@ -3443,7 +3454,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>169</v>
       </c>
@@ -3478,7 +3489,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>170</v>
       </c>
@@ -3513,7 +3524,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -3548,7 +3559,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>172</v>
       </c>
@@ -3583,7 +3594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>173</v>
       </c>
@@ -3618,7 +3629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>174</v>
       </c>
@@ -3653,7 +3664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>175</v>
       </c>
@@ -3688,7 +3699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -3723,7 +3734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>177</v>
       </c>
@@ -3758,7 +3769,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>178</v>
       </c>
@@ -3793,7 +3804,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -3828,7 +3839,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -3863,7 +3874,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>181</v>
       </c>
@@ -3898,7 +3909,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>182</v>
       </c>
@@ -3933,7 +3944,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>183</v>
       </c>
@@ -3968,7 +3979,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>184</v>
       </c>
@@ -4003,7 +4014,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>185</v>
       </c>
@@ -4038,7 +4049,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>186</v>
       </c>
@@ -4073,7 +4084,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>187</v>
       </c>
@@ -4108,7 +4119,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>188</v>
       </c>
@@ -4143,7 +4154,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -4178,7 +4189,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>190</v>
       </c>
@@ -4213,7 +4224,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -4248,7 +4259,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>192</v>
       </c>
@@ -4283,7 +4294,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -4318,7 +4329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>194</v>
       </c>
@@ -4353,7 +4364,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>195</v>
       </c>
@@ -4388,7 +4399,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -4423,7 +4434,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -4458,7 +4469,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>198</v>
       </c>
@@ -4493,7 +4504,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>199</v>
       </c>
@@ -4528,7 +4539,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>200</v>
       </c>
@@ -4563,7 +4574,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>201</v>
       </c>
@@ -4598,7 +4609,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>202</v>
       </c>
@@ -4633,7 +4644,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -4668,7 +4679,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>204</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>205</v>
       </c>
@@ -4738,7 +4749,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>206</v>
       </c>
@@ -4773,7 +4784,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -4808,7 +4819,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -4843,7 +4854,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -4878,7 +4889,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>210</v>
       </c>
@@ -4913,7 +4924,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>212</v>
       </c>
@@ -4948,7 +4959,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>213</v>
       </c>
@@ -4983,7 +4994,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>214</v>
       </c>
@@ -5018,7 +5029,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>215</v>
       </c>
@@ -5053,7 +5064,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>216</v>
       </c>
@@ -5088,7 +5099,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>217</v>
       </c>
@@ -5123,7 +5134,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>218</v>
       </c>
@@ -5158,7 +5169,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>219</v>
       </c>
@@ -5193,7 +5204,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>220</v>
       </c>
@@ -5228,7 +5239,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>221</v>
       </c>
@@ -5263,7 +5274,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>222</v>
       </c>
@@ -5298,7 +5309,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>223</v>
       </c>
@@ -5333,7 +5344,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>224</v>
       </c>
@@ -5368,7 +5379,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>225</v>
       </c>
@@ -5403,7 +5414,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>226</v>
       </c>
@@ -5438,7 +5449,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -5473,7 +5484,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>228</v>
       </c>
@@ -5508,7 +5519,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>229</v>
       </c>
@@ -5543,7 +5554,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>230</v>
       </c>
@@ -5578,7 +5589,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>231</v>
       </c>
@@ -5613,7 +5624,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>232</v>
       </c>
@@ -5648,7 +5659,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>233</v>
       </c>
@@ -5683,7 +5694,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>234</v>
       </c>
@@ -5718,7 +5729,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>235</v>
       </c>
@@ -5753,7 +5764,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>236</v>
       </c>
@@ -5788,7 +5799,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>237</v>
       </c>
@@ -5823,7 +5834,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>238</v>
       </c>
@@ -5858,7 +5869,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>211</v>
       </c>
@@ -5893,7 +5904,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>239</v>
       </c>
@@ -5928,7 +5939,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>240</v>
       </c>
@@ -5963,7 +5974,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>241</v>
       </c>
@@ -5998,7 +6009,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>242</v>
       </c>
@@ -6033,7 +6044,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>243</v>
       </c>
@@ -6068,7 +6079,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>244</v>
       </c>
@@ -6103,7 +6114,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>245</v>
       </c>
@@ -6138,7 +6149,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>246</v>
       </c>
@@ -6173,7 +6184,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>247</v>
       </c>
@@ -6208,7 +6219,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>342</v>
       </c>
@@ -6243,7 +6254,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>248</v>
       </c>
@@ -6278,7 +6289,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>249</v>
       </c>
@@ -6313,7 +6324,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>250</v>
       </c>
@@ -6348,7 +6359,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>251</v>
       </c>
@@ -6383,7 +6394,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>252</v>
       </c>
@@ -6418,7 +6429,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>253</v>
       </c>
@@ -6453,7 +6464,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>254</v>
       </c>
@@ -6488,7 +6499,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>255</v>
       </c>
@@ -6523,7 +6534,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>256</v>
       </c>
@@ -6558,7 +6569,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>257</v>
       </c>
@@ -6593,7 +6604,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>258</v>
       </c>
@@ -6628,7 +6639,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -6663,7 +6674,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -6698,7 +6709,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>261</v>
       </c>
@@ -6733,7 +6744,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>262</v>
       </c>
@@ -6768,7 +6779,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>263</v>
       </c>
@@ -6803,7 +6814,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>264</v>
       </c>
@@ -6838,7 +6849,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>265</v>
       </c>
@@ -6873,7 +6884,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>266</v>
       </c>
@@ -6908,7 +6919,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>267</v>
       </c>
@@ -6943,7 +6954,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>268</v>
       </c>
@@ -6978,7 +6989,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>269</v>
       </c>
@@ -7013,7 +7024,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>270</v>
       </c>
@@ -7048,7 +7059,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>271</v>
       </c>
@@ -7083,7 +7094,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>272</v>
       </c>
@@ -7118,7 +7129,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>273</v>
       </c>
@@ -7153,7 +7164,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>274</v>
       </c>
@@ -7188,7 +7199,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>275</v>
       </c>
@@ -7223,7 +7234,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>276</v>
       </c>
@@ -7258,7 +7269,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>277</v>
       </c>
@@ -7293,7 +7304,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>278</v>
       </c>
@@ -7328,7 +7339,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>279</v>
       </c>
@@ -7363,7 +7374,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>280</v>
       </c>
@@ -7398,7 +7409,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>281</v>
       </c>
@@ -7433,7 +7444,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>282</v>
       </c>
@@ -7468,7 +7479,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>283</v>
       </c>
@@ -7503,7 +7514,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>284</v>
       </c>
@@ -7538,7 +7549,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>285</v>
       </c>
@@ -7573,7 +7584,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>286</v>
       </c>
@@ -7608,7 +7619,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>287</v>
       </c>
@@ -7643,7 +7654,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>288</v>
       </c>
@@ -7678,7 +7689,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>289</v>
       </c>
@@ -7713,7 +7724,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>290</v>
       </c>
@@ -7748,7 +7759,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>291</v>
       </c>
@@ -7783,7 +7794,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>292</v>
       </c>
@@ -7818,7 +7829,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>293</v>
       </c>
@@ -7853,7 +7864,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>294</v>
       </c>
@@ -7888,7 +7899,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>295</v>
       </c>
@@ -7923,7 +7934,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>296</v>
       </c>
@@ -7958,7 +7969,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>297</v>
       </c>
@@ -7993,7 +8004,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>298</v>
       </c>
@@ -8028,7 +8039,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>299</v>
       </c>
@@ -8063,7 +8074,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>300</v>
       </c>
@@ -8098,7 +8109,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>301</v>
       </c>
@@ -8133,7 +8144,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>302</v>
       </c>
@@ -8168,7 +8179,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>303</v>
       </c>
@@ -8203,7 +8214,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>304</v>
       </c>
@@ -8238,7 +8249,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>305</v>
       </c>
@@ -8273,7 +8284,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>306</v>
       </c>
@@ -8308,7 +8319,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>307</v>
       </c>
@@ -8343,7 +8354,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>308</v>
       </c>
@@ -8378,7 +8389,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>309</v>
       </c>
@@ -8413,7 +8424,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>310</v>
       </c>
@@ -8448,7 +8459,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>311</v>
       </c>
@@ -8483,7 +8494,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>312</v>
       </c>
@@ -8518,7 +8529,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>313</v>
       </c>
@@ -8553,7 +8564,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>314</v>
       </c>
@@ -8588,7 +8599,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>315</v>
       </c>
@@ -8623,7 +8634,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>316</v>
       </c>
@@ -8658,7 +8669,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>317</v>
       </c>
@@ -8693,7 +8704,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>318</v>
       </c>
@@ -8728,7 +8739,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>319</v>
       </c>
@@ -8763,7 +8774,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>320</v>
       </c>
@@ -8798,7 +8809,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>321</v>
       </c>
@@ -8833,7 +8844,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>322</v>
       </c>
@@ -8868,7 +8879,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>323</v>
       </c>
@@ -8903,7 +8914,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>324</v>
       </c>
@@ -8938,7 +8949,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>325</v>
       </c>
@@ -8973,7 +8984,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>326</v>
       </c>
@@ -9008,7 +9019,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>327</v>
       </c>
@@ -9043,7 +9054,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>328</v>
       </c>
@@ -9078,7 +9089,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>329</v>
       </c>
@@ -9113,7 +9124,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>330</v>
       </c>
@@ -9148,7 +9159,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>331</v>
       </c>
@@ -9183,7 +9194,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>332</v>
       </c>
@@ -9218,7 +9229,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>333</v>
       </c>
@@ -9253,7 +9264,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>334</v>
       </c>
@@ -9288,7 +9299,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>335</v>
       </c>
@@ -9323,7 +9334,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>336</v>
       </c>
@@ -9358,7 +9369,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>337</v>
       </c>
@@ -9393,7 +9404,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>338</v>
       </c>

</xml_diff>